<commit_message>
new data and paper outline. quicksort still segfaulting on sorted input
</commit_message>
<xml_diff>
--- a/executionTimeData.xlsx
+++ b/executionTimeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharp\Desktop\School\2024\S2024\CSCI2226-DatastructuresAndAlgorithms\SortingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF14C44-05D1-4EAF-8B6B-3335A75BD6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DAABAD-E1CE-4ABD-87EF-76A877ECE522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,6 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,7 +560,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6647,8 +6647,8 @@
   </sheetPr>
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6667,33 +6667,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="28" t="s">
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="31"/>
     </row>
     <row r="2" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -6705,13 +6705,13 @@
       <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -6779,10 +6779,10 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="21">
@@ -6842,31 +6842,31 @@
         <v>22</v>
       </c>
       <c r="U3" s="23">
-        <v>1</v>
+        <v>2.1277601000000002</v>
       </c>
       <c r="V3" s="23">
-        <v>1</v>
+        <v>2.1578704000000002</v>
       </c>
       <c r="W3" s="23">
-        <v>1</v>
+        <v>2.1883205999999999</v>
       </c>
       <c r="X3" s="23">
-        <v>1</v>
+        <v>2.2097034999999998</v>
       </c>
       <c r="Y3" s="23">
-        <v>1</v>
+        <v>2.2142867000000002</v>
       </c>
       <c r="Z3" s="24">
         <f>AVERAGE(U3:Y3)</f>
-        <v>1</v>
+        <v>2.1795882600000001</v>
       </c>
       <c r="AA3" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="37"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="5">
         <v>100000</v>
       </c>
@@ -6929,32 +6929,32 @@
         <v>4.0771005259065198</v>
       </c>
       <c r="U4" s="13">
-        <v>1</v>
+        <v>8.5239635000000007</v>
       </c>
       <c r="V4" s="13">
-        <v>1</v>
+        <v>8.7298425000000002</v>
       </c>
       <c r="W4" s="13">
-        <v>1</v>
+        <v>8.7067104999999998</v>
       </c>
       <c r="X4" s="13">
-        <v>1</v>
+        <v>8.7705885000000006</v>
       </c>
       <c r="Y4" s="13">
-        <v>1</v>
+        <v>8.8558328999999993</v>
       </c>
       <c r="Z4" s="17">
         <f t="shared" ref="Z4:Z38" si="2">AVERAGE(U4:Y4)</f>
-        <v>1</v>
+        <v>8.7173875799999987</v>
       </c>
       <c r="AA4" s="13">
         <f>Z4/Z3</f>
-        <v>1</v>
+        <v>3.9995570447787228</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="37"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="5">
         <v>175000</v>
       </c>
@@ -7017,32 +7017,32 @@
         <v>3.046987215426074</v>
       </c>
       <c r="U5" s="13">
-        <v>1</v>
+        <v>26.128881199999999</v>
       </c>
       <c r="V5" s="13">
-        <v>1</v>
+        <v>26.100149999999999</v>
       </c>
       <c r="W5" s="13">
-        <v>1</v>
+        <v>26.571992900000001</v>
       </c>
       <c r="X5" s="13">
-        <v>1</v>
+        <v>26.698799399999999</v>
       </c>
       <c r="Y5" s="13">
-        <v>1</v>
+        <v>26.7329179</v>
       </c>
       <c r="Z5" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>26.446548279999995</v>
       </c>
       <c r="AA5" s="13">
         <f t="shared" ref="AA5:AA8" si="7">Z5/Z4</f>
-        <v>1</v>
+        <v>3.0337699267467926</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="5">
         <v>300000</v>
       </c>
@@ -7105,32 +7105,32 @@
         <v>2.966214588801388</v>
       </c>
       <c r="U6" s="13">
-        <v>1</v>
+        <v>80.369632699999997</v>
       </c>
       <c r="V6" s="13">
-        <v>1</v>
+        <v>81.282623999999998</v>
       </c>
       <c r="W6" s="13">
-        <v>1</v>
+        <v>81.875777400000004</v>
       </c>
       <c r="X6" s="13">
-        <v>1</v>
+        <v>81.930251799999994</v>
       </c>
       <c r="Y6" s="13">
-        <v>1</v>
+        <v>80.685685699999993</v>
       </c>
       <c r="Z6" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>81.228794319999992</v>
       </c>
       <c r="AA6" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>3.0714327427533772</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A7" s="37"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="5">
         <v>425000</v>
       </c>
@@ -7193,32 +7193,32 @@
         <v>2.0101659471503854</v>
       </c>
       <c r="U7" s="13">
-        <v>1</v>
+        <v>164.48117250000001</v>
       </c>
       <c r="V7" s="13">
-        <v>1</v>
+        <v>156.06983550000001</v>
       </c>
       <c r="W7" s="13">
-        <v>1</v>
+        <v>156.6599014</v>
       </c>
       <c r="X7" s="13">
-        <v>1</v>
+        <v>159.75662489999999</v>
       </c>
       <c r="Y7" s="13">
-        <v>1</v>
+        <v>160.46309980000001</v>
       </c>
       <c r="Z7" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>159.48612682000001</v>
       </c>
       <c r="AA7" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.963418614730462</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="38"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="6">
         <v>550000</v>
       </c>
@@ -7280,35 +7280,35 @@
         <f t="shared" si="6"/>
         <v>1.6944446769219377</v>
       </c>
-      <c r="U8" s="41">
-        <v>1</v>
-      </c>
-      <c r="V8" s="41">
-        <v>1</v>
-      </c>
-      <c r="W8" s="41">
-        <v>1</v>
-      </c>
-      <c r="X8" s="41">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="41">
-        <v>1</v>
+      <c r="U8" s="28">
+        <v>270.1389375</v>
+      </c>
+      <c r="V8" s="28">
+        <v>259.9608983</v>
+      </c>
+      <c r="W8" s="28">
+        <v>263.655912</v>
+      </c>
+      <c r="X8" s="28">
+        <v>259.37422320000002</v>
+      </c>
+      <c r="Y8" s="28">
+        <v>260.890017</v>
       </c>
       <c r="Z8" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>262.80399759999995</v>
       </c>
       <c r="AA8" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.6478172919492053</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="21">
@@ -7368,31 +7368,31 @@
         <v>22</v>
       </c>
       <c r="U9" s="23">
-        <v>1</v>
+        <v>0.8898258</v>
       </c>
       <c r="V9" s="23">
-        <v>1</v>
+        <v>0.86695129999999998</v>
       </c>
       <c r="W9" s="23">
-        <v>1</v>
+        <v>0.90057010000000004</v>
       </c>
       <c r="X9" s="23">
-        <v>1</v>
+        <v>0.87598430000000005</v>
       </c>
       <c r="Y9" s="23">
-        <v>1</v>
+        <v>0.88712849999999999</v>
       </c>
       <c r="Z9" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.8840920000000001</v>
       </c>
       <c r="AA9" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="5">
         <v>100000</v>
       </c>
@@ -7455,32 +7455,32 @@
         <v>3.9831024333170126</v>
       </c>
       <c r="U10" s="13">
-        <v>1</v>
+        <v>3.5842619</v>
       </c>
       <c r="V10" s="13">
-        <v>1</v>
+        <v>3.4624703999999999</v>
       </c>
       <c r="W10" s="13">
-        <v>1</v>
+        <v>3.4977830000000001</v>
       </c>
       <c r="X10" s="13">
-        <v>1</v>
+        <v>3.5559403000000001</v>
       </c>
       <c r="Y10" s="13">
-        <v>1</v>
+        <v>3.6623644</v>
       </c>
       <c r="Z10" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.5525640000000003</v>
       </c>
       <c r="AA10" s="13">
         <f>Z10/Z9</f>
-        <v>1</v>
+        <v>4.0183193604285528</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A11" s="37"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="5">
         <v>175000</v>
       </c>
@@ -7543,32 +7543,32 @@
         <v>3.1932060605497714</v>
       </c>
       <c r="U11" s="13">
-        <v>1</v>
+        <v>10.950929199999999</v>
       </c>
       <c r="V11" s="13">
-        <v>1</v>
+        <v>11.0006199</v>
       </c>
       <c r="W11" s="13">
-        <v>1</v>
+        <v>10.9295607</v>
       </c>
       <c r="X11" s="13">
-        <v>1</v>
+        <v>10.917384699999999</v>
       </c>
       <c r="Y11" s="13">
-        <v>1</v>
+        <v>10.881433400000001</v>
       </c>
       <c r="Z11" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10.935985580000001</v>
       </c>
       <c r="AA11" s="13">
         <f t="shared" ref="AA11:AA14" si="10">Z11/Z10</f>
-        <v>1</v>
+        <v>3.0783359793095917</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A12" s="37"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="5">
         <v>300000</v>
       </c>
@@ -7631,32 +7631,32 @@
         <v>2.9135916517369367</v>
       </c>
       <c r="U12" s="13">
-        <v>1</v>
+        <v>32.401791500000002</v>
       </c>
       <c r="V12" s="13">
-        <v>1</v>
+        <v>31.927645399999999</v>
       </c>
       <c r="W12" s="13">
-        <v>1</v>
+        <v>32.691670600000002</v>
       </c>
       <c r="X12" s="13">
-        <v>1</v>
+        <v>32.610088500000003</v>
       </c>
       <c r="Y12" s="13">
-        <v>1</v>
+        <v>32.730861500000003</v>
       </c>
       <c r="Z12" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>32.4724115</v>
       </c>
       <c r="AA12" s="13">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2.96931732969604</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="5">
         <v>425000</v>
       </c>
@@ -7719,32 +7719,32 @@
         <v>2.0210193374347081</v>
       </c>
       <c r="U13" s="13">
-        <v>1</v>
+        <v>64.892133400000006</v>
       </c>
       <c r="V13" s="13">
-        <v>1</v>
+        <v>63.723070499999999</v>
       </c>
       <c r="W13" s="13">
-        <v>1</v>
+        <v>63.819937600000003</v>
       </c>
       <c r="X13" s="13">
-        <v>1</v>
+        <v>64.925417100000004</v>
       </c>
       <c r="Y13" s="13">
-        <v>1</v>
+        <v>64.699296700000005</v>
       </c>
       <c r="Z13" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>64.411971059999999</v>
       </c>
       <c r="AA13" s="13">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.9835906261535272</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="38"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="6">
         <v>550000</v>
       </c>
@@ -7807,34 +7807,34 @@
         <v>1.6780426103059489</v>
       </c>
       <c r="U14" s="20">
-        <v>1</v>
+        <v>110.4811869</v>
       </c>
       <c r="V14" s="20">
-        <v>1</v>
+        <v>109.1348787</v>
       </c>
       <c r="W14" s="20">
-        <v>1</v>
+        <v>107.7225772</v>
       </c>
       <c r="X14" s="20">
-        <v>1</v>
+        <v>113.56047649999999</v>
       </c>
       <c r="Y14" s="20">
-        <v>1</v>
+        <v>113.26993659999999</v>
       </c>
       <c r="Z14" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>110.83381118</v>
       </c>
       <c r="AA14" s="13">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.7207020582673658</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="21">
@@ -7894,31 +7894,31 @@
         <v>22</v>
       </c>
       <c r="U15" s="13">
-        <v>1</v>
+        <v>1.0876026000000001</v>
       </c>
       <c r="V15" s="13">
-        <v>1</v>
+        <v>1.1079417</v>
       </c>
       <c r="W15" s="13">
-        <v>1</v>
+        <v>1.1222122999999999</v>
       </c>
       <c r="X15" s="13">
-        <v>1</v>
+        <v>1.1188175</v>
       </c>
       <c r="Y15" s="13">
-        <v>1</v>
+        <v>1.1501872</v>
       </c>
       <c r="Z15" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.1173522599999999</v>
       </c>
       <c r="AA15" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="5">
         <v>100000</v>
       </c>
@@ -7981,32 +7981,32 @@
         <v>1.4951259138911455</v>
       </c>
       <c r="U16" s="13">
-        <v>1</v>
+        <v>4.2625006000000001</v>
       </c>
       <c r="V16" s="13">
-        <v>1</v>
+        <v>4.2710279</v>
       </c>
       <c r="W16" s="13">
-        <v>1</v>
+        <v>4.2785130999999996</v>
       </c>
       <c r="X16" s="13">
-        <v>1</v>
+        <v>4.414866</v>
       </c>
       <c r="Y16" s="13">
-        <v>1</v>
+        <v>4.4334512999999998</v>
       </c>
       <c r="Z16" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.3320717799999997</v>
       </c>
       <c r="AA16" s="13">
         <f>Z16/Z15</f>
-        <v>1</v>
+        <v>3.8770868732122135</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="5">
         <v>175000</v>
       </c>
@@ -8069,32 +8069,32 @@
         <v>1.8139092637870142</v>
       </c>
       <c r="U17" s="13">
-        <v>1</v>
+        <v>13.047761400000001</v>
       </c>
       <c r="V17" s="13">
-        <v>1</v>
+        <v>13.382273700000001</v>
       </c>
       <c r="W17" s="13">
-        <v>1</v>
+        <v>13.371559899999999</v>
       </c>
       <c r="X17" s="13">
-        <v>1</v>
+        <v>13.411699499999999</v>
       </c>
       <c r="Y17" s="13">
-        <v>1</v>
+        <v>13.5598308</v>
       </c>
       <c r="Z17" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>13.35462506</v>
       </c>
       <c r="AA17" s="13">
         <f t="shared" ref="AA17:AA20" si="15">Z17/Z16</f>
-        <v>1</v>
+        <v>3.0827340215493848</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="5">
         <v>300000</v>
       </c>
@@ -8157,32 +8157,32 @@
         <v>1.9583645349707952</v>
       </c>
       <c r="U18" s="13">
-        <v>1</v>
+        <v>40.860741099999998</v>
       </c>
       <c r="V18" s="13">
-        <v>1</v>
+        <v>41.030571199999997</v>
       </c>
       <c r="W18" s="13">
-        <v>1</v>
+        <v>41.041561199999997</v>
       </c>
       <c r="X18" s="13">
-        <v>1</v>
+        <v>41.311354899999998</v>
       </c>
       <c r="Y18" s="13">
-        <v>1</v>
+        <v>41.462623999999998</v>
       </c>
       <c r="Z18" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>41.141370479999999</v>
       </c>
       <c r="AA18" s="13">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>3.0806833059826841</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A19" s="37"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="5">
         <v>425000</v>
       </c>
@@ -8245,32 +8245,32 @@
         <v>1.2263306821657998</v>
       </c>
       <c r="U19" s="13">
-        <v>1</v>
+        <v>81.621755300000004</v>
       </c>
       <c r="V19" s="13">
-        <v>1</v>
+        <v>83.471276399999994</v>
       </c>
       <c r="W19" s="13">
-        <v>1</v>
+        <v>82.813548100000006</v>
       </c>
       <c r="X19" s="13">
-        <v>1</v>
+        <v>82.310394000000002</v>
       </c>
       <c r="Y19" s="13">
-        <v>1</v>
+        <v>81.754149699999999</v>
       </c>
       <c r="Z19" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>82.394224699999995</v>
       </c>
       <c r="AA19" s="13">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>2.0027097721514697</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="6">
         <v>550000</v>
       </c>
@@ -8332,35 +8332,35 @@
         <f t="shared" si="14"/>
         <v>1.2481993077858502</v>
       </c>
-      <c r="U20" s="41">
-        <v>1</v>
-      </c>
-      <c r="V20" s="41">
-        <v>1</v>
-      </c>
-      <c r="W20" s="41">
-        <v>1</v>
-      </c>
-      <c r="X20" s="41">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="41">
-        <v>1</v>
+      <c r="U20" s="28">
+        <v>141.31139619999999</v>
+      </c>
+      <c r="V20" s="28">
+        <v>139.90312180000001</v>
+      </c>
+      <c r="W20" s="28">
+        <v>132.35164900000001</v>
+      </c>
+      <c r="X20" s="28">
+        <v>133.54685269999999</v>
+      </c>
+      <c r="Y20" s="28">
+        <v>132.62209770000001</v>
       </c>
       <c r="Z20" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>135.94702348000001</v>
       </c>
       <c r="AA20" s="13">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>1.6499581612059275</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="21">
@@ -8420,31 +8420,31 @@
         <v>22</v>
       </c>
       <c r="U21" s="23">
-        <v>1</v>
+        <v>2.7335600000000002E-2</v>
       </c>
       <c r="V21" s="23">
-        <v>1</v>
+        <v>1.83158E-2</v>
       </c>
       <c r="W21" s="23">
-        <v>1</v>
+        <v>2.06678E-2</v>
       </c>
       <c r="X21" s="23">
-        <v>1</v>
+        <v>1.8178400000000001E-2</v>
       </c>
       <c r="Y21" s="23">
-        <v>1</v>
+        <v>2.05493E-2</v>
       </c>
       <c r="Z21" s="24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.1009380000000001E-2</v>
       </c>
       <c r="AA21" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A22" s="37"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="5">
         <v>100000</v>
       </c>
@@ -8507,32 +8507,32 @@
         <v>1.3844928070277056</v>
       </c>
       <c r="U22" s="13">
-        <v>1</v>
+        <v>3.6842899999999998E-2</v>
       </c>
       <c r="V22" s="13">
-        <v>1</v>
+        <v>4.2576900000000001E-2</v>
       </c>
       <c r="W22" s="13">
-        <v>1</v>
+        <v>3.6690800000000003E-2</v>
       </c>
       <c r="X22" s="13">
-        <v>1</v>
+        <v>4.1958599999999999E-2</v>
       </c>
       <c r="Y22" s="13">
-        <v>1</v>
+        <v>3.7886200000000002E-2</v>
       </c>
       <c r="Z22" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.9191080000000003E-2</v>
       </c>
       <c r="AA22" s="13">
         <f>Z22/Z21</f>
-        <v>1</v>
+        <v>1.8654086888808714</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A23" s="37"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="5">
         <v>175000</v>
       </c>
@@ -8595,32 +8595,32 @@
         <v>1.703328553205846</v>
       </c>
       <c r="U23" s="13">
-        <v>1</v>
+        <v>6.6186400000000006E-2</v>
       </c>
       <c r="V23" s="13">
-        <v>1</v>
+        <v>7.2501599999999999E-2</v>
       </c>
       <c r="W23" s="13">
-        <v>1</v>
+        <v>6.4273800000000006E-2</v>
       </c>
       <c r="X23" s="13">
-        <v>1</v>
+        <v>7.2145799999999996E-2</v>
       </c>
       <c r="Y23" s="13">
-        <v>1</v>
+        <v>6.6806599999999994E-2</v>
       </c>
       <c r="Z23" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6.838284E-2</v>
       </c>
       <c r="AA23" s="13">
         <f t="shared" ref="AA23:AA26" si="20">Z23/Z22</f>
-        <v>1</v>
+        <v>1.7448572481289109</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="5">
         <v>300000</v>
       </c>
@@ -8683,32 +8683,32 @@
         <v>1.7643616140089393</v>
       </c>
       <c r="U24" s="13">
-        <v>1</v>
+        <v>0.12178</v>
       </c>
       <c r="V24" s="13">
-        <v>1</v>
+        <v>0.110601</v>
       </c>
       <c r="W24" s="13">
-        <v>1</v>
+        <v>0.12419289999999999</v>
       </c>
       <c r="X24" s="13">
-        <v>1</v>
+        <v>0.1101193</v>
       </c>
       <c r="Y24" s="13">
-        <v>1</v>
+        <v>0.1250452</v>
       </c>
       <c r="Z24" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.11834768</v>
       </c>
       <c r="AA24" s="13">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>1.7306634237478291</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A25" s="37"/>
-      <c r="B25" s="34"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="5">
         <v>425000</v>
       </c>
@@ -8771,32 +8771,32 @@
         <v>1.4289742762673263</v>
       </c>
       <c r="U25" s="13">
-        <v>1</v>
+        <v>0.15834970000000001</v>
       </c>
       <c r="V25" s="13">
-        <v>1</v>
+        <v>0.1731722</v>
       </c>
       <c r="W25" s="13">
-        <v>1</v>
+        <v>0.1545792</v>
       </c>
       <c r="X25" s="13">
-        <v>1</v>
+        <v>0.17828830000000001</v>
       </c>
       <c r="Y25" s="13">
-        <v>1</v>
+        <v>0.15979070000000001</v>
       </c>
       <c r="Z25" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.16483602000000003</v>
       </c>
       <c r="AA25" s="13">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>1.392811587012099</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="38"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="6">
         <v>550000</v>
       </c>
@@ -8859,34 +8859,34 @@
         <v>1.3059731617562851</v>
       </c>
       <c r="U26" s="20">
-        <v>1</v>
+        <v>0.2284928</v>
       </c>
       <c r="V26" s="20">
-        <v>1</v>
+        <v>0.20143269999999999</v>
       </c>
       <c r="W26" s="20">
-        <v>1</v>
+        <v>0.2281531</v>
       </c>
       <c r="X26" s="20">
-        <v>1</v>
+        <v>0.20309740000000001</v>
       </c>
       <c r="Y26" s="20">
-        <v>1</v>
+        <v>0.2260112</v>
       </c>
       <c r="Z26" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.21743744000000001</v>
       </c>
       <c r="AA26" s="13">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>1.3191136257718428</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="21">
@@ -8969,8 +8969,8 @@
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A28" s="37"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="5">
         <v>100000</v>
       </c>
@@ -9057,8 +9057,8 @@
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A29" s="37"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="5">
         <v>175000</v>
       </c>
@@ -9145,8 +9145,8 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A30" s="37"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="5">
         <v>300000</v>
       </c>
@@ -9233,8 +9233,8 @@
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A31" s="37"/>
-      <c r="B31" s="34"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="5">
         <v>425000</v>
       </c>
@@ -9321,8 +9321,8 @@
       </c>
     </row>
     <row r="32" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="38"/>
-      <c r="B32" s="35"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="6">
         <v>550000</v>
       </c>
@@ -9409,10 +9409,10 @@
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="34" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="11">
@@ -9472,31 +9472,31 @@
         <v>22</v>
       </c>
       <c r="U33" s="23">
-        <v>1</v>
+        <v>2.0267000000000002E-3</v>
       </c>
       <c r="V33" s="23">
-        <v>1</v>
+        <v>1.5097000000000001E-3</v>
       </c>
       <c r="W33" s="23">
-        <v>1</v>
+        <v>1.4984E-3</v>
       </c>
       <c r="X33" s="23">
-        <v>1</v>
+        <v>2.1448000000000001E-3</v>
       </c>
       <c r="Y33" s="23">
-        <v>1</v>
+        <v>1.7941000000000001E-3</v>
       </c>
       <c r="Z33" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.7947400000000002E-3</v>
       </c>
       <c r="AA33" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A34" s="37"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="5">
         <v>100000</v>
       </c>
@@ -9559,32 +9559,32 @@
         <v>2.0754802546846367</v>
       </c>
       <c r="U34" s="13">
-        <v>1</v>
+        <v>3.2815000000000001E-3</v>
       </c>
       <c r="V34" s="13">
-        <v>1</v>
+        <v>3.2460000000000002E-3</v>
       </c>
       <c r="W34" s="13">
-        <v>1</v>
+        <v>3.2948000000000001E-3</v>
       </c>
       <c r="X34" s="13">
-        <v>1</v>
+        <v>3.0866000000000001E-3</v>
       </c>
       <c r="Y34" s="13">
-        <v>1</v>
+        <v>3.4102E-3</v>
       </c>
       <c r="Z34" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.2638199999999997E-3</v>
       </c>
       <c r="AA34" s="13">
         <f>Z34/Z33</f>
-        <v>1</v>
+        <v>1.8185475333474483</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A35" s="37"/>
-      <c r="B35" s="34"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="5">
         <v>175000</v>
       </c>
@@ -9647,32 +9647,32 @@
         <v>1.7807193112791162</v>
       </c>
       <c r="U35" s="13">
-        <v>1</v>
+        <v>7.4361000000000002E-3</v>
       </c>
       <c r="V35" s="13">
-        <v>1</v>
+        <v>5.5846000000000003E-3</v>
       </c>
       <c r="W35" s="13">
-        <v>1</v>
+        <v>5.6917000000000001E-3</v>
       </c>
       <c r="X35" s="13">
-        <v>1</v>
+        <v>5.9611999999999998E-3</v>
       </c>
       <c r="Y35" s="13">
-        <v>1</v>
+        <v>6.6128000000000003E-3</v>
       </c>
       <c r="Z35" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6.2572799999999996E-3</v>
       </c>
       <c r="AA35" s="13">
         <f t="shared" ref="AA35:AA38" si="30">Z35/Z34</f>
-        <v>1</v>
+        <v>1.9171645495155982</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A36" s="37"/>
-      <c r="B36" s="34"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="5">
         <v>300000</v>
       </c>
@@ -9735,32 +9735,32 @@
         <v>1.7741299002164508</v>
       </c>
       <c r="U36" s="13">
-        <v>1</v>
+        <v>1.0884400000000001E-2</v>
       </c>
       <c r="V36" s="13">
-        <v>1</v>
+        <v>1.0806899999999999E-2</v>
       </c>
       <c r="W36" s="13">
-        <v>1</v>
+        <v>1.0020899999999999E-2</v>
       </c>
       <c r="X36" s="13">
-        <v>1</v>
+        <v>1.1213900000000001E-2</v>
       </c>
       <c r="Y36" s="13">
-        <v>1</v>
+        <v>1.09687E-2</v>
       </c>
       <c r="Z36" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0778959999999999E-2</v>
       </c>
       <c r="AA36" s="13">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>1.7226270839725886</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A37" s="37"/>
-      <c r="B37" s="34"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="5">
         <v>425000</v>
       </c>
@@ -9823,32 +9823,32 @@
         <v>1.4080555962850971</v>
       </c>
       <c r="U37" s="13">
-        <v>1</v>
+        <v>1.5783700000000001E-2</v>
       </c>
       <c r="V37" s="13">
-        <v>1</v>
+        <v>1.52129E-2</v>
       </c>
       <c r="W37" s="13">
-        <v>1</v>
+        <v>1.4568599999999999E-2</v>
       </c>
       <c r="X37" s="13">
-        <v>1</v>
+        <v>1.50096E-2</v>
       </c>
       <c r="Y37" s="13">
-        <v>1</v>
+        <v>1.5428799999999999E-2</v>
       </c>
       <c r="Z37" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5200720000000001E-2</v>
       </c>
       <c r="AA37" s="13">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>1.4102213942718038</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="38"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6">
         <v>550000</v>
       </c>
@@ -9911,27 +9911,27 @@
         <v>1.3612621817038666</v>
       </c>
       <c r="U38" s="20">
-        <v>1</v>
+        <v>2.00632E-2</v>
       </c>
       <c r="V38" s="20">
-        <v>1</v>
+        <v>2.0836E-2</v>
       </c>
       <c r="W38" s="20">
-        <v>1</v>
+        <v>2.04212E-2</v>
       </c>
       <c r="X38" s="20">
-        <v>1</v>
+        <v>2.06912E-2</v>
       </c>
       <c r="Y38" s="20">
-        <v>1</v>
+        <v>2.0744599999999998E-2</v>
       </c>
       <c r="Z38" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.0551239999999998E-2</v>
       </c>
       <c r="AA38" s="10">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>1.3519912214684566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>